<commit_message>
Full Automation Complete upload #5
Made some fixes to the sending of the report part of the automation. The full process now runs as expected.
</commit_message>
<xml_diff>
--- a/BlizzardAutomation/Data/Input/09072020.xlsx
+++ b/BlizzardAutomation/Data/Input/09072020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\UiPath\BlizzardAutomation\Data\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B03E57B-4A4D-41B0-93D6-D8F67793FCE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31F5F2E9-431F-4808-80A2-00F9A51B9569}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23040" yWindow="1836" windowWidth="23016" windowHeight="10560" xr2:uid="{2E9F313C-B456-42AE-AB8A-5FDB477C2952}"/>
   </bookViews>
@@ -433,7 +433,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF0D9F3B-99D8-44FE-B2EF-A84958447EAA}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -493,6 +493,84 @@
         <v>0.06</v>
       </c>
       <c r="H4">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>0.50209490740740736</v>
+      </c>
+      <c r="B5">
+        <v>71.760000000000005</v>
+      </c>
+      <c r="C5">
+        <v>72.819999999999993</v>
+      </c>
+      <c r="D5">
+        <v>71.22</v>
+      </c>
+      <c r="E5">
+        <v>71.7</v>
+      </c>
+      <c r="F5">
+        <v>71.760000000000005</v>
+      </c>
+      <c r="G5">
+        <v>0.06</v>
+      </c>
+      <c r="H5">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>0.51635416666666667</v>
+      </c>
+      <c r="B6">
+        <v>71.760000000000005</v>
+      </c>
+      <c r="C6">
+        <v>72.819999999999993</v>
+      </c>
+      <c r="D6">
+        <v>71.22</v>
+      </c>
+      <c r="E6">
+        <v>71.7</v>
+      </c>
+      <c r="F6">
+        <v>71.760000000000005</v>
+      </c>
+      <c r="G6">
+        <v>0.06</v>
+      </c>
+      <c r="H6">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>0.53057870370370364</v>
+      </c>
+      <c r="B7">
+        <v>71.760000000000005</v>
+      </c>
+      <c r="C7">
+        <v>72.819999999999993</v>
+      </c>
+      <c r="D7">
+        <v>71.22</v>
+      </c>
+      <c r="E7">
+        <v>71.7</v>
+      </c>
+      <c r="F7">
+        <v>71.760000000000005</v>
+      </c>
+      <c r="G7">
+        <v>0.06</v>
+      </c>
+      <c r="H7">
         <v>0.08</v>
       </c>
     </row>
@@ -521,7 +599,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E458FBB2-BD9F-4F47-A93E-8CCDDDF9A16B}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -581,6 +659,84 @@
         <v>0.83</v>
       </c>
       <c r="H4">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>0.50012731481481476</v>
+      </c>
+      <c r="B5">
+        <v>135.61000000000001</v>
+      </c>
+      <c r="C5">
+        <v>136.34</v>
+      </c>
+      <c r="D5">
+        <v>134.51</v>
+      </c>
+      <c r="E5">
+        <v>134.78</v>
+      </c>
+      <c r="F5">
+        <v>135.61000000000001</v>
+      </c>
+      <c r="G5">
+        <v>0.83</v>
+      </c>
+      <c r="H5">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>0.51503472222222224</v>
+      </c>
+      <c r="B6">
+        <v>135.61000000000001</v>
+      </c>
+      <c r="C6">
+        <v>136.34</v>
+      </c>
+      <c r="D6">
+        <v>134.51</v>
+      </c>
+      <c r="E6">
+        <v>134.78</v>
+      </c>
+      <c r="F6">
+        <v>135.61000000000001</v>
+      </c>
+      <c r="G6">
+        <v>0.83</v>
+      </c>
+      <c r="H6">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>0.5285185185185185</v>
+      </c>
+      <c r="B7">
+        <v>135.61000000000001</v>
+      </c>
+      <c r="C7">
+        <v>136.34</v>
+      </c>
+      <c r="D7">
+        <v>134.51</v>
+      </c>
+      <c r="E7">
+        <v>134.78</v>
+      </c>
+      <c r="F7">
+        <v>135.61000000000001</v>
+      </c>
+      <c r="G7">
+        <v>0.83</v>
+      </c>
+      <c r="H7">
         <v>0.62</v>
       </c>
     </row>
@@ -609,7 +765,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8ED1099-F0F8-40F1-9655-F7CCC1E154D9}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -672,6 +828,84 @@
         <v>1.19</v>
       </c>
     </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>0.49677083333333333</v>
+      </c>
+      <c r="B5">
+        <v>412.8</v>
+      </c>
+      <c r="C5">
+        <v>409</v>
+      </c>
+      <c r="D5">
+        <v>398.62</v>
+      </c>
+      <c r="E5">
+        <v>394.87</v>
+      </c>
+      <c r="F5">
+        <v>412.8</v>
+      </c>
+      <c r="G5">
+        <v>4.16</v>
+      </c>
+      <c r="H5">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>0.51265046296296302</v>
+      </c>
+      <c r="B6">
+        <v>413.52</v>
+      </c>
+      <c r="C6">
+        <v>409</v>
+      </c>
+      <c r="D6">
+        <v>398.62</v>
+      </c>
+      <c r="E6">
+        <v>394.87</v>
+      </c>
+      <c r="F6">
+        <v>413.52</v>
+      </c>
+      <c r="G6">
+        <v>4.88</v>
+      </c>
+      <c r="H6">
+        <v>1.19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>0.52491898148148153</v>
+      </c>
+      <c r="B7">
+        <v>414.89</v>
+      </c>
+      <c r="C7">
+        <v>409</v>
+      </c>
+      <c r="D7">
+        <v>398.62</v>
+      </c>
+      <c r="E7">
+        <v>394.87</v>
+      </c>
+      <c r="F7">
+        <v>414.89</v>
+      </c>
+      <c r="G7">
+        <v>6.25</v>
+      </c>
+      <c r="H7">
+        <v>1.53</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -679,7 +913,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A72EBC0-35A7-4B81-9D13-F5CEF4A0853C}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -740,6 +974,84 @@
       </c>
       <c r="H4">
         <v>0.95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>0.49525462962962963</v>
+      </c>
+      <c r="B5">
+        <v>214.2</v>
+      </c>
+      <c r="C5">
+        <v>213.26</v>
+      </c>
+      <c r="D5">
+        <v>208.69</v>
+      </c>
+      <c r="E5">
+        <v>208.25</v>
+      </c>
+      <c r="F5">
+        <v>214.2</v>
+      </c>
+      <c r="G5">
+        <v>1.37</v>
+      </c>
+      <c r="H5">
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>0.51143518518518516</v>
+      </c>
+      <c r="B6">
+        <v>214.54</v>
+      </c>
+      <c r="C6">
+        <v>213.26</v>
+      </c>
+      <c r="D6">
+        <v>208.69</v>
+      </c>
+      <c r="E6">
+        <v>208.25</v>
+      </c>
+      <c r="F6">
+        <v>214.54</v>
+      </c>
+      <c r="G6">
+        <v>1.71</v>
+      </c>
+      <c r="H6">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>0.52339120370370373</v>
+      </c>
+      <c r="B7">
+        <v>215.14</v>
+      </c>
+      <c r="C7">
+        <v>213.26</v>
+      </c>
+      <c r="D7">
+        <v>208.69</v>
+      </c>
+      <c r="E7">
+        <v>208.25</v>
+      </c>
+      <c r="F7">
+        <v>215.14</v>
+      </c>
+      <c r="G7">
+        <v>2.31</v>
+      </c>
+      <c r="H7">
+        <v>1.0900000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>